<commit_message>
Updated To Eliminate and To Add list for PCOS. Noted the assumptions. Added additional logging.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/input/IngredientsAndComorbidities.xlsx
+++ b/src/test/resources/TestData/input/IngredientsAndComorbidities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eswar\git\SmartScrapper2023\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eswar\git\SmartScrapper2023\src\test\resources\TestData\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2289AB-FC92-49E7-B6F8-27332A43B75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E55F11-B314-43D1-A381-F8F494D6790A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="210">
   <si>
     <t>Diabetes</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Iodized salt</t>
   </si>
   <si>
-    <t>Sugary foods (sweets, icecreams) and beverages (soda, juices)</t>
-  </si>
-  <si>
     <t>Sweet potatoes</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
   </si>
   <si>
     <t>Cakes, pastries</t>
-  </si>
-  <si>
-    <t>Seed oils- vegetable oil, soybean oil, canola oil, rapeseed oil, sunflower oil, safflower oil</t>
   </si>
   <si>
     <t>Jams</t>
@@ -596,12 +590,78 @@
   <si>
     <t>mustard greens</t>
   </si>
+  <si>
+    <t>sweets</t>
+  </si>
+  <si>
+    <t>icecreams</t>
+  </si>
+  <si>
+    <t>juices</t>
+  </si>
+  <si>
+    <t>juice</t>
+  </si>
+  <si>
+    <t>icecream</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>vegetable oil</t>
+  </si>
+  <si>
+    <t>soybean oil</t>
+  </si>
+  <si>
+    <t>canola oil</t>
+  </si>
+  <si>
+    <t>rapeseed oil</t>
+  </si>
+  <si>
+    <t>sunflower oil</t>
+  </si>
+  <si>
+    <t>safflower oil</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>Berries (raspberries, blackberries, strawberries)</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Oranges and Citrus Fruits</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Sweet Potatoes</t>
+  </si>
+  <si>
+    <t>Brussels Sprouts</t>
+  </si>
+  <si>
+    <t>Peas</t>
+  </si>
+  <si>
+    <t>Artichokes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -628,6 +688,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -671,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -693,6 +759,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,8 +982,8 @@
   </sheetPr>
   <dimension ref="A1:Z1029"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1082,7 @@
     </row>
     <row r="3" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -1022,10 +1091,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
@@ -1057,7 +1126,7 @@
     </row>
     <row r="4" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -1066,18 +1135,20 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1099,7 +1170,7 @@
     </row>
     <row r="5" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1108,18 +1179,20 @@
         <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1141,10 +1214,10 @@
     </row>
     <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>21</v>
@@ -1153,15 +1226,17 @@
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="11" t="s">
+        <v>201</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1183,10 +1258,10 @@
     </row>
     <row r="7" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>26</v>
@@ -1195,15 +1270,17 @@
         <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1237,15 +1314,17 @@
         <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1270,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>37</v>
@@ -1279,15 +1358,17 @@
         <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1317,12 +1398,14 @@
         <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1350,7 +1433,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>38</v>
@@ -1361,7 +1444,12 @@
       <c r="F11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="G11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1389,18 +1477,23 @@
         <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="G12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>205</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1422,25 +1515,29 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>206</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1462,25 +1559,29 @@
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1502,16 +1603,16 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>28</v>
@@ -1519,8 +1620,12 @@
       <c r="F15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1542,25 +1647,29 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1582,25 +1691,29 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>208</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1622,24 +1735,26 @@
     </row>
     <row r="18" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="11" t="s">
+        <v>209</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1661,23 +1776,21 @@
     </row>
     <row r="19" spans="1:26" ht="64.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="7"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1700,20 +1813,20 @@
     </row>
     <row r="20" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="7"/>
@@ -1738,20 +1851,20 @@
     </row>
     <row r="21" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
@@ -1776,10 +1889,10 @@
     </row>
     <row r="22" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>24</v>
@@ -1789,7 +1902,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="7"/>
@@ -1814,22 +1927,22 @@
     </row>
     <row r="23" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="1"/>
@@ -1853,18 +1966,18 @@
     </row>
     <row r="24" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>
@@ -1889,19 +2002,19 @@
     </row>
     <row r="25" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="1"/>
@@ -1925,17 +2038,17 @@
     </row>
     <row r="26" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7"/>
@@ -1960,14 +2073,14 @@
     </row>
     <row r="27" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
@@ -1992,14 +2105,14 @@
     </row>
     <row r="28" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="7"/>
@@ -2024,14 +2137,14 @@
     </row>
     <row r="29" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="7"/>
@@ -2056,13 +2169,13 @@
     </row>
     <row r="30" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>18</v>
@@ -2089,16 +2202,16 @@
     </row>
     <row r="31" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="1"/>
@@ -2122,17 +2235,17 @@
     </row>
     <row r="32" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="1"/>
@@ -2156,11 +2269,11 @@
     </row>
     <row r="33" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E33" s="7"/>
       <c r="G33" s="6" t="s">
@@ -2188,11 +2301,11 @@
     </row>
     <row r="34" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2221,13 +2334,13 @@
     </row>
     <row r="35" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="6"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="G35" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="1"/>
@@ -2251,13 +2364,13 @@
     </row>
     <row r="36" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="G36" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="1"/>
@@ -2281,13 +2394,13 @@
     </row>
     <row r="37" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="G37" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="1"/>
@@ -2311,13 +2424,15 @@
     </row>
     <row r="38" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>197</v>
+      </c>
       <c r="H38" s="7"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2340,14 +2455,16 @@
     </row>
     <row r="39" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="G39" s="6" t="s">
+        <v>194</v>
+      </c>
       <c r="H39" s="7"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2370,14 +2487,16 @@
     </row>
     <row r="40" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="G40" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="H40" s="7"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2400,14 +2519,16 @@
     </row>
     <row r="41" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="G41" s="6" t="s">
+        <v>196</v>
+      </c>
       <c r="H41" s="7"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2430,14 +2551,16 @@
     </row>
     <row r="42" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="G42" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="H42" s="7"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2460,14 +2583,14 @@
     </row>
     <row r="43" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="6" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="1"/>
@@ -2491,13 +2614,12 @@
     </row>
     <row r="44" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2520,7 +2642,7 @@
     </row>
     <row r="45" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B45" s="7"/>
       <c r="D45" s="7"/>
@@ -2549,7 +2671,7 @@
     </row>
     <row r="46" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B46" s="7"/>
       <c r="D46" s="7"/>
@@ -2578,7 +2700,7 @@
     </row>
     <row r="47" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="7"/>
       <c r="D47" s="7"/>
@@ -2607,7 +2729,7 @@
     </row>
     <row r="48" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B48" s="7"/>
       <c r="D48" s="7"/>
@@ -2636,7 +2758,7 @@
     </row>
     <row r="49" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="6"/>
@@ -2666,7 +2788,7 @@
     </row>
     <row r="50" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="6"/>
@@ -2696,7 +2818,7 @@
     </row>
     <row r="51" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="6"/>
@@ -2726,7 +2848,7 @@
     </row>
     <row r="52" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="6"/>
@@ -2756,7 +2878,7 @@
     </row>
     <row r="53" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="6"/>
@@ -2786,7 +2908,7 @@
     </row>
     <row r="54" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="6"/>
@@ -2816,7 +2938,7 @@
     </row>
     <row r="55" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B55" s="7"/>
       <c r="D55" s="7"/>
@@ -2845,7 +2967,7 @@
     </row>
     <row r="56" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B56" s="7"/>
       <c r="D56" s="7"/>
@@ -2874,7 +2996,7 @@
     </row>
     <row r="57" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B57" s="7"/>
       <c r="D57" s="7"/>
@@ -2903,7 +3025,7 @@
     </row>
     <row r="58" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B58" s="7"/>
       <c r="D58" s="7"/>
@@ -2932,7 +3054,7 @@
     </row>
     <row r="59" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B59" s="7"/>
       <c r="D59" s="7"/>
@@ -2961,7 +3083,7 @@
     </row>
     <row r="60" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -2991,7 +3113,7 @@
     </row>
     <row r="61" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -3021,7 +3143,7 @@
     </row>
     <row r="62" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -3051,7 +3173,7 @@
     </row>
     <row r="63" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -3081,7 +3203,7 @@
     </row>
     <row r="64" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3111,7 +3233,7 @@
     </row>
     <row r="65" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -3141,7 +3263,7 @@
     </row>
     <row r="66" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -3171,7 +3293,7 @@
     </row>
     <row r="67" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -3201,7 +3323,7 @@
     </row>
     <row r="68" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -3231,7 +3353,7 @@
     </row>
     <row r="69" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -3261,7 +3383,7 @@
     </row>
     <row r="70" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -3291,7 +3413,7 @@
     </row>
     <row r="71" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -3321,7 +3443,7 @@
     </row>
     <row r="72" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>

</xml_diff>